<commit_message>
Scenariusz 4 - wersja 1
</commit_message>
<xml_diff>
--- a/Sprawozdania/Scenariusz 3/Wyniki do scenariusza 3 - PSI.xlsx
+++ b/Sprawozdania/Scenariusz 3/Wyniki do scenariusza 3 - PSI.xlsx
@@ -782,6 +782,49 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Arkusz1!$I$3:$I$22</c:f>
@@ -930,11 +973,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="268496736"/>
-        <c:axId val="268498416"/>
+        <c:axId val="274300944"/>
+        <c:axId val="274301504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="268496736"/>
+        <c:axId val="274300944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1058,12 +1101,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="268498416"/>
+        <c:crossAx val="274301504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="268498416"/>
+        <c:axId val="274301504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1187,7 +1230,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="268496736"/>
+        <c:crossAx val="274300944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1529,11 +1572,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="272351072"/>
-        <c:axId val="272351632"/>
+        <c:axId val="277118912"/>
+        <c:axId val="277119472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="272351072"/>
+        <c:axId val="277118912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1590,12 +1633,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="272351632"/>
+        <c:crossAx val="277119472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="272351632"/>
+        <c:axId val="277119472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1652,7 +1695,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="272351072"/>
+        <c:crossAx val="277118912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2021,11 +2064,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="272355552"/>
-        <c:axId val="272356112"/>
+        <c:axId val="277551584"/>
+        <c:axId val="277552144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="272355552"/>
+        <c:axId val="277551584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2082,12 +2125,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="272356112"/>
+        <c:crossAx val="277552144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="272356112"/>
+        <c:axId val="277552144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2144,7 +2187,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="272355552"/>
+        <c:crossAx val="277551584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2238,6 +2281,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2346,11 +2390,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="272830336"/>
-        <c:axId val="272830896"/>
+        <c:axId val="277554944"/>
+        <c:axId val="277555504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="272830336"/>
+        <c:axId val="277554944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2407,12 +2451,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="272830896"/>
+        <c:crossAx val="277555504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="272830896"/>
+        <c:axId val="277555504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2469,7 +2513,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="272830336"/>
+        <c:crossAx val="277554944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2558,6 +2602,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2666,11 +2711,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="272833136"/>
-        <c:axId val="272833696"/>
+        <c:axId val="277557744"/>
+        <c:axId val="276610816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="272833136"/>
+        <c:axId val="277557744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2727,12 +2772,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="272833696"/>
+        <c:crossAx val="276610816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="272833696"/>
+        <c:axId val="276610816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2789,7 +2834,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="272833136"/>
+        <c:crossAx val="277557744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2961,6 +3006,20 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Arkusz1!$I$3:$I$22</c:f>
@@ -3109,11 +3168,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="267542528"/>
-        <c:axId val="267543088"/>
+        <c:axId val="274540624"/>
+        <c:axId val="274543424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="267542528"/>
+        <c:axId val="274540624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3237,12 +3296,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="267543088"/>
+        <c:crossAx val="274543424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="267543088"/>
+        <c:axId val="274543424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3366,7 +3425,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="267542528"/>
+        <c:crossAx val="274540624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3538,6 +3597,20 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Arkusz1!$I$3:$I$22</c:f>
@@ -3686,11 +3759,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="267545328"/>
-        <c:axId val="267545888"/>
+        <c:axId val="274547344"/>
+        <c:axId val="276048384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="267545328"/>
+        <c:axId val="274547344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3814,12 +3887,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="267545888"/>
+        <c:crossAx val="276048384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="267545888"/>
+        <c:axId val="276048384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3943,7 +4016,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="267545328"/>
+        <c:crossAx val="274547344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4115,6 +4188,20 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Arkusz1!$I$3:$I$22</c:f>
@@ -4263,11 +4350,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="267548128"/>
-        <c:axId val="267548688"/>
+        <c:axId val="276050624"/>
+        <c:axId val="276051184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="267548128"/>
+        <c:axId val="276050624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4391,12 +4478,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="267548688"/>
+        <c:crossAx val="276051184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="267548688"/>
+        <c:axId val="276051184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4520,7 +4607,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="267548128"/>
+        <c:crossAx val="276050624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4692,6 +4779,20 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Arkusz1!$I$3:$I$22</c:f>
@@ -4840,11 +4941,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="267677664"/>
-        <c:axId val="267678224"/>
+        <c:axId val="276053424"/>
+        <c:axId val="276053984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="267677664"/>
+        <c:axId val="276053424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4968,12 +5069,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="267678224"/>
+        <c:crossAx val="276053984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="267678224"/>
+        <c:axId val="276053984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5097,7 +5198,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="267677664"/>
+        <c:crossAx val="276053424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5337,6 +5438,20 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Arkusz1!$I$3:$I$22</c:f>
@@ -5485,11 +5600,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="267680464"/>
-        <c:axId val="267681024"/>
+        <c:axId val="276447872"/>
+        <c:axId val="276448432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="267680464"/>
+        <c:axId val="276447872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5613,12 +5728,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="267681024"/>
+        <c:crossAx val="276448432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="267681024"/>
+        <c:axId val="276448432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5742,7 +5857,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="267680464"/>
+        <c:crossAx val="276447872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5982,6 +6097,20 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Arkusz1!$I$3:$I$22</c:f>
@@ -6130,11 +6259,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="267683264"/>
-        <c:axId val="267683824"/>
+        <c:axId val="276450672"/>
+        <c:axId val="276451232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="267683264"/>
+        <c:axId val="276450672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6258,12 +6387,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="267683824"/>
+        <c:crossAx val="276451232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="267683824"/>
+        <c:axId val="276451232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6387,7 +6516,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="267683264"/>
+        <c:crossAx val="276450672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6559,6 +6688,20 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Arkusz1!$I$3:$I$22</c:f>
@@ -6707,11 +6850,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="267899408"/>
-        <c:axId val="267899968"/>
+        <c:axId val="276453472"/>
+        <c:axId val="276454032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="267899408"/>
+        <c:axId val="276453472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6835,12 +6978,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="267899968"/>
+        <c:crossAx val="276454032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="267899968"/>
+        <c:axId val="276454032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6964,7 +7107,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="267899408"/>
+        <c:crossAx val="276453472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7136,6 +7279,20 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Arkusz1!$I$3:$I$22</c:f>
@@ -7284,11 +7441,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="267902208"/>
-        <c:axId val="267902768"/>
+        <c:axId val="277114992"/>
+        <c:axId val="277115552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="267902208"/>
+        <c:axId val="277114992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7412,12 +7569,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="267902768"/>
+        <c:crossAx val="277115552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="267902768"/>
+        <c:axId val="277115552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7541,7 +7698,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="267902208"/>
+        <c:crossAx val="277114992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -15899,7 +16056,7 @@
   <dimension ref="A1:CD46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Scenariusz 4 - wersja 2
</commit_message>
<xml_diff>
--- a/Sprawozdania/Scenariusz 3/Wyniki do scenariusza 3 - PSI.xlsx
+++ b/Sprawozdania/Scenariusz 3/Wyniki do scenariusza 3 - PSI.xlsx
@@ -973,11 +973,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="274300944"/>
-        <c:axId val="274301504"/>
+        <c:axId val="299850144"/>
+        <c:axId val="299850704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="274300944"/>
+        <c:axId val="299850144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1101,12 +1101,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="274301504"/>
+        <c:crossAx val="299850704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="274301504"/>
+        <c:axId val="299850704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1230,7 +1230,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="274300944"/>
+        <c:crossAx val="299850144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1572,11 +1572,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="277118912"/>
-        <c:axId val="277119472"/>
+        <c:axId val="300487744"/>
+        <c:axId val="300488304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="277118912"/>
+        <c:axId val="300487744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1633,12 +1633,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="277119472"/>
+        <c:crossAx val="300488304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="277119472"/>
+        <c:axId val="300488304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1695,7 +1695,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="277118912"/>
+        <c:crossAx val="300487744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2064,11 +2064,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="277551584"/>
-        <c:axId val="277552144"/>
+        <c:axId val="300753696"/>
+        <c:axId val="300754256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="277551584"/>
+        <c:axId val="300753696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2125,12 +2125,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="277552144"/>
+        <c:crossAx val="300754256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="277552144"/>
+        <c:axId val="300754256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2187,7 +2187,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="277551584"/>
+        <c:crossAx val="300753696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2281,7 +2281,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2390,11 +2389,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="277554944"/>
-        <c:axId val="277555504"/>
+        <c:axId val="300757056"/>
+        <c:axId val="300757616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="277554944"/>
+        <c:axId val="300757056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2451,12 +2450,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="277555504"/>
+        <c:crossAx val="300757616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="277555504"/>
+        <c:axId val="300757616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2513,7 +2512,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="277554944"/>
+        <c:crossAx val="300757056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2602,7 +2601,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2711,11 +2709,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="277557744"/>
-        <c:axId val="276610816"/>
+        <c:axId val="300759856"/>
+        <c:axId val="300876512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="277557744"/>
+        <c:axId val="300759856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2772,12 +2770,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276610816"/>
+        <c:crossAx val="300876512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="276610816"/>
+        <c:axId val="300876512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2834,7 +2832,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="277557744"/>
+        <c:crossAx val="300759856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3168,11 +3166,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="274540624"/>
-        <c:axId val="274543424"/>
+        <c:axId val="299852944"/>
+        <c:axId val="299853504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="274540624"/>
+        <c:axId val="299852944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3296,12 +3294,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="274543424"/>
+        <c:crossAx val="299853504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="274543424"/>
+        <c:axId val="299853504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3425,7 +3423,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="274540624"/>
+        <c:crossAx val="299852944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3759,11 +3757,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="274547344"/>
-        <c:axId val="276048384"/>
+        <c:axId val="299855744"/>
+        <c:axId val="297218032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="274547344"/>
+        <c:axId val="299855744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3887,12 +3885,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276048384"/>
+        <c:crossAx val="297218032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="276048384"/>
+        <c:axId val="297218032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4016,7 +4014,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="274547344"/>
+        <c:crossAx val="299855744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4350,11 +4348,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="276050624"/>
-        <c:axId val="276051184"/>
+        <c:axId val="297220272"/>
+        <c:axId val="297220832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="276050624"/>
+        <c:axId val="297220272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4478,12 +4476,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276051184"/>
+        <c:crossAx val="297220832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="276051184"/>
+        <c:axId val="297220832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4607,7 +4605,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276050624"/>
+        <c:crossAx val="297220272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4941,11 +4939,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="276053424"/>
-        <c:axId val="276053984"/>
+        <c:axId val="297223072"/>
+        <c:axId val="297223632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="276053424"/>
+        <c:axId val="297223072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5069,12 +5067,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276053984"/>
+        <c:crossAx val="297223632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="276053984"/>
+        <c:axId val="297223632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5198,7 +5196,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276053424"/>
+        <c:crossAx val="297223072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5600,11 +5598,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="276447872"/>
-        <c:axId val="276448432"/>
+        <c:axId val="297676016"/>
+        <c:axId val="297676576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="276447872"/>
+        <c:axId val="297676016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5728,12 +5726,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276448432"/>
+        <c:crossAx val="297676576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="276448432"/>
+        <c:axId val="297676576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5857,7 +5855,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276447872"/>
+        <c:crossAx val="297676016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6259,11 +6257,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="276450672"/>
-        <c:axId val="276451232"/>
+        <c:axId val="297678816"/>
+        <c:axId val="297679376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="276450672"/>
+        <c:axId val="297678816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6387,12 +6385,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276451232"/>
+        <c:crossAx val="297679376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="276451232"/>
+        <c:axId val="297679376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6516,7 +6514,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276450672"/>
+        <c:crossAx val="297678816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6850,11 +6848,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="276453472"/>
-        <c:axId val="276454032"/>
+        <c:axId val="297681616"/>
+        <c:axId val="297682176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="276453472"/>
+        <c:axId val="297681616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6978,12 +6976,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276454032"/>
+        <c:crossAx val="297682176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="276454032"/>
+        <c:axId val="297682176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7107,7 +7105,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276453472"/>
+        <c:crossAx val="297681616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7441,11 +7439,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="277114992"/>
-        <c:axId val="277115552"/>
+        <c:axId val="300483824"/>
+        <c:axId val="300484384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="277114992"/>
+        <c:axId val="300483824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7569,12 +7567,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="277115552"/>
+        <c:crossAx val="300484384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="277115552"/>
+        <c:axId val="300484384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7698,7 +7696,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="277114992"/>
+        <c:crossAx val="300483824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -16056,7 +16054,7 @@
   <dimension ref="A1:CD46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>